<commit_message>
close #3 checking duplicate is now working
</commit_message>
<xml_diff>
--- a/test/data/test_duplicate.xlsx
+++ b/test/data/test_duplicate.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t xml:space="preserve">307-8705-45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert</t>
   </si>
 </sst>
 </file>
@@ -231,7 +234,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
@@ -483,6 +486,32 @@
         <v>98206337</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>14851</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>98206337</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>